<commit_message>
Changes marked OK in matrix
See change matrix
</commit_message>
<xml_diff>
--- a/201806 - FtCollins/Comments_Resolution_GeoTIFF_draft06062018.xlsx
+++ b/201806 - FtCollins/Comments_Resolution_GeoTIFF_draft06062018.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedhabermann/GitRepositories/geotiff/201806 - FtCollins/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479146AB-08F9-C147-AE05-73BABA90CD68}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18915" windowHeight="7740"/>
+    <workbookView xWindow="1560" yWindow="4660" windowWidth="41960" windowHeight="22700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$29</definedName>
+  </definedNames>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>Even Rouault</t>
   </si>
@@ -421,12 +430,45 @@
   <si>
     <t>Fixing GeoTIFF to be able to unambiguously define a user-defined CRS is not a trivial exercise.</t>
   </si>
+  <si>
+    <t>0e</t>
+  </si>
+  <si>
+    <t>0f</t>
+  </si>
+  <si>
+    <t>5e</t>
+  </si>
+  <si>
+    <t>7a</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Removed one requirement. New requirement has ID = http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.EPSGGeographic
+_GeographicTypeGeoKey values in the range_ _1024-32766 SHALL be geographic 
+2D or 3D EPSG CRS codes_</t>
+  </si>
+  <si>
+    <t>these two requirements were merged in a single VerticalCSTypeGeoKey.EPSGValues requirement</t>
+  </si>
+  <si>
+    <t>Removed http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.angular and changed wording of 
+GeogLinearUnitsGeoKey values in the range 1024-32766 SHALL be EPSG Unit Of Measure (UOM) Codes that express linear units</t>
+  </si>
+  <si>
+    <t>Removed http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.angular
+VerticalUnitsGeoKey values in the range 1024-32766 SHALL be EPSG__Unit of Measure (UOM) Codes
+and reworded http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.linear +
+_VerticalUnitsGeoKey values in the range 1024-32766 SHALL be EPSG Unit of Measure (UOM) Codes that express linear units_</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,7 +477,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -443,14 +492,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF009900"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -492,44 +541,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,12 +598,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -587,7 +648,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -620,9 +681,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -655,6 +733,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -830,587 +925,643 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="9" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="40.6640625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.83203125" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="H1" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="6">
         <v>43243</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="251.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" ht="251.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>43243</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="315" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="336" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>43243</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:8" ht="400.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>43244</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="345" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" ht="368" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="405" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="6">
         <v>43242</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="H8" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="171" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="6">
         <v>43243</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="15" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <f>A8+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="6">
         <v>43242</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="H10" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <f t="shared" ref="A11:A28" si="0">A10+1</f>
         <v>3</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="6">
         <v>43242</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+    <row r="12" spans="1:8" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="6">
         <v>43242</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="H12" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="155.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="6">
         <v>43242</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="11" t="s">
+      <c r="F13" s="7"/>
+      <c r="G13" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="6">
         <v>43243</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="11" t="s">
+      <c r="F14" s="7"/>
+      <c r="G14" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" ht="208" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="6">
         <v>43243</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14" t="s">
+      <c r="F15" s="7"/>
+      <c r="G15" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" ht="272" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="6">
         <v>43243</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="14" t="s">
+      <c r="F16" s="7"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" ht="240" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="F17" s="7"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" ht="208" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <f>A13+1</f>
         <v>6</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="6">
         <v>43242</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="11" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="360.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="H18" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="360.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="6">
         <v>43242</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="7"/>
+      <c r="G19" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13" t="s">
+    <row r="20" spans="1:8" ht="128" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="15" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
         <v>8</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="6">
         <v>43242</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="10" t="s">
+      <c r="F21" s="7"/>
+      <c r="G21" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" ht="128" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="6">
         <v>43243</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="11" t="s">
+      <c r="F22" s="7"/>
+      <c r="G22" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" ht="256" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" ht="300" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="F23" s="7"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" ht="320" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="F24" s="7"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" ht="112" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="6">
         <v>43243</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="15" t="s">
+      <c r="F25" s="7"/>
+      <c r="G25" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="6">
         <v>43256</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13" t="s">
+      <c r="F26" s="7"/>
+      <c r="G26" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="6">
         <v>43256</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="18" t="s">
+      <c r="F27" s="7"/>
+      <c r="G27" s="12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="399.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" ht="399.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="6">
         <v>43256</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="10" t="s">
+      <c r="F28" s="7"/>
+      <c r="G28" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13" t="s">
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>16</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="11"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H29" xr:uid="{7976A120-1FDE-1240-873F-B1F96F8B8E17}">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter val="*OK*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" display="http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.angular"/>
+    <hyperlink ref="E10" r:id="rId1" display="http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.angular" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
@@ -1418,24 +1569,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>